<commit_message>
Updated the file based on class feedback
</commit_message>
<xml_diff>
--- a/Constraints.xlsx
+++ b/Constraints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="520" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="520" windowWidth="25720" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="97">
   <si>
     <t>Constraint</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Michael T</t>
   </si>
   <si>
-    <t>Navigate and orient itself (turn, stabilize, etc.)</t>
-  </si>
-  <si>
     <t>Shiva</t>
   </si>
   <si>
@@ -195,21 +192,12 @@
     <t>Limited on board eletrical magnetic interference</t>
   </si>
   <si>
-    <t>Dampening Vibration</t>
-  </si>
-  <si>
     <t>Trajectory planner</t>
   </si>
   <si>
     <t>Hui</t>
   </si>
   <si>
-    <t>Provide provably saft and complete algorithms on board</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Prioritizing high probability areas in the building first</t>
   </si>
   <si>
@@ -252,15 +240,9 @@
     <t>Quick return function in case of emergency situation</t>
   </si>
   <si>
-    <t>Drop/Impact Resistance</t>
-  </si>
-  <si>
     <t>Josh C</t>
   </si>
   <si>
-    <t>Interchangable Payload</t>
-  </si>
-  <si>
     <t>Adequate fatigue life on fatigue sensitive components</t>
   </si>
   <si>
@@ -279,20 +261,55 @@
     <t>Low</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sufficient maneuverability to navigate small openings - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>How is this different than #4?</t>
-    </r>
-  </si>
-  <si>
-    <t>unknown</t>
+    <t xml:space="preserve">Schedule </t>
+  </si>
+  <si>
+    <t>Distinguishing between hot/cold items such as live/dead persons and pipes</t>
+  </si>
+  <si>
+    <t>Weather tolerant - Texas proof, Nashville winter proof, humidity, rain</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Interchangable Payload/power supplies</t>
+  </si>
+  <si>
+    <t>Josh C, Rebecca</t>
+  </si>
+  <si>
+    <t>Drop/Impact Resistance/protection of critical systems such as propellers</t>
+  </si>
+  <si>
+    <t>Josh C, Mike W</t>
+  </si>
+  <si>
+    <t>Fatigue mitigation/Dampening Vibration</t>
+  </si>
+  <si>
+    <t>Franco, Josh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> track mapped/visited areas, prioritization of areas</t>
+  </si>
+  <si>
+    <t>Shiva,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rebecca, Dan C, and Nolan</t>
+  </si>
+  <si>
+    <t>Provide provably safe and complete algorithms on board</t>
+  </si>
+  <si>
+    <t>Flight stablization</t>
+  </si>
+  <si>
+    <t>Navigate, orient itself (turn, etc.),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sufficient maneuverability to navigate small openings </t>
   </si>
 </sst>
 </file>
@@ -302,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -342,18 +359,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -365,7 +383,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -495,8 +513,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -506,8 +540,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="145">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +609,14 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -636,6 +681,14 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -965,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -980,7 +1033,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1000,7 +1053,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -1039,10 +1092,10 @@
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1">
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="3">
@@ -1051,64 +1104,62 @@
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1">
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" s="2" customFormat="1">
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="3">
-        <v>41648</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+        <v>41652</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="2" customFormat="1">
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="3">
-        <v>41648</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3">
         <v>41648</v>
       </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1">
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="3">
@@ -1117,10 +1168,10 @@
     </row>
     <row r="12" spans="1:7" s="2" customFormat="1">
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3">
@@ -1129,10 +1180,10 @@
     </row>
     <row r="13" spans="1:7" s="2" customFormat="1">
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3">
@@ -1141,20 +1192,22 @@
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1">
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3">
+        <v>41648</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1">
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="3">
@@ -1162,29 +1215,31 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1">
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="3">
-        <v>41648</v>
-      </c>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1">
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="3">
@@ -1193,40 +1248,38 @@
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1">
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="E20" s="3">
+        <v>41648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
-        <v>41648</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1">
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="3">
@@ -1235,10 +1288,10 @@
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1">
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="3">
@@ -1247,15 +1300,13 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1">
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="3">
-        <v>41648</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1">
       <c r="B25" s="1"/>
@@ -1263,51 +1314,52 @@
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:7" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
-        <v>82</v>
-      </c>
+    <row r="26" spans="1:7">
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="3">
         <v>41648</v>
       </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1">
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="3">
         <v>41648</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1">
+    <row r="28" spans="1:7">
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="3">
         <v>41648</v>
       </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1">
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="3">
@@ -1316,14 +1368,14 @@
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1">
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="3">
-        <v>41652</v>
+        <v>41648</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1">
@@ -1332,34 +1384,39 @@
       <c r="D31" s="1"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:7" s="2" customFormat="1">
+    <row r="32" spans="1:7">
+      <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="3">
-        <v>41652</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="2" customFormat="1">
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>41648</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="3">
-        <v>41648</v>
-      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1">
+      <c r="A34" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="3">
@@ -1367,118 +1424,125 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="3">
+        <v>41648</v>
+      </c>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1">
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="3">
         <v>41648</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" s="2" customFormat="1">
       <c r="B37" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="3">
         <v>41648</v>
       </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1">
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="3">
-        <v>41648</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" s="2" customFormat="1">
-      <c r="B40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="1" t="s">
+        <v>41652</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="6" customFormat="1">
+      <c r="B40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="7">
+        <v>41648</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" s="2" customFormat="1">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" s="2" customFormat="1">
+      <c r="B43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="3">
+        <v>41648</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="B44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="3">
-        <v>41648</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="2" customFormat="1">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" s="2" customFormat="1">
-      <c r="B42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="3">
-        <v>41648</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="2" customFormat="1">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="3"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="3">
+        <v>41648</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="3">
-        <v>41648</v>
-      </c>
+      <c r="E45" s="3"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="3">
@@ -1487,98 +1551,79 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" s="2" customFormat="1">
       <c r="B47" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="3">
         <v>41648</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="B48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>42</v>
-      </c>
+    </row>
+    <row r="48" spans="1:7" s="2" customFormat="1">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="3">
-        <v>41648</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" s="2" customFormat="1">
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="B50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="E49" s="3">
+        <v>41648</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="2" customFormat="1">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="3">
-        <v>41652</v>
-      </c>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7">
       <c r="B52" s="1" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="3"/>
+      <c r="E52" s="3">
+        <v>41648</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="3"/>
+      <c r="E53" s="3">
+        <v>41648</v>
+      </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="B54" s="1" t="s">
-        <v>36</v>
+      <c r="B54" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="3">
@@ -1589,10 +1634,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="B55" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="3">
@@ -1603,35 +1648,37 @@
     </row>
     <row r="56" spans="1:7">
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="3">
-        <v>41652</v>
-      </c>
+      <c r="E56" s="3"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:7">
       <c r="B57" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="3">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D58" s="1"/>
       <c r="E58" s="3"/>
       <c r="F58" s="1"/>
@@ -1639,15 +1686,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="3">
-        <v>41648</v>
-      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
@@ -1660,14 +1705,11 @@
       <c r="G60" s="1"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="B61" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="3">
@@ -1677,53 +1719,72 @@
       <c r="G61" s="1"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="4"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D62" s="1"/>
-      <c r="E62" s="3"/>
+      <c r="E62" s="3">
+        <v>41648</v>
+      </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="1:7">
       <c r="B63" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="3">
+        <v>41652</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="3">
+        <v>41648</v>
+      </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="B65" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="3"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
     <row r="66" spans="1:7">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="3"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="3">
@@ -1733,36 +1794,45 @@
       <c r="G67" s="1"/>
     </row>
     <row r="68" spans="1:7">
+      <c r="A68" s="4"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="3"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="D69" s="1"/>
-      <c r="E69" s="3"/>
+      <c r="B69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="D70" s="1"/>
-      <c r="E70" s="3"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="D71" s="1"/>
-      <c r="E71" s="3"/>
+      <c r="B71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="D72" s="1"/>
-      <c r="E72" s="3"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7">
-      <c r="D73" s="1"/>
-      <c r="E73" s="3"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
@@ -1773,6 +1843,8 @@
       <c r="G74" s="1"/>
     </row>
     <row r="75" spans="1:7">
+      <c r="D75" s="1"/>
+      <c r="E75" s="3"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
@@ -1789,10 +1861,14 @@
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="1:7">
+      <c r="D78" s="1"/>
+      <c r="E78" s="3"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="1:7">
+      <c r="D79" s="1"/>
+      <c r="E79" s="3"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
@@ -1801,24 +1877,48 @@
       <c r="G80" s="1"/>
     </row>
     <row r="81" spans="2:7">
+      <c r="D81" s="1"/>
+      <c r="E81" s="3"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="3"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="3"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>